<commit_message>
Update IRAP procedural parameters and stimuli.xlsx
</commit_message>
<xml_diff>
--- a/method/IRAP procedural parameters and stimuli.xlsx
+++ b/method/IRAP procedural parameters and stimuli.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ian/git/generic-pattern-among-irap-effects/method/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5575FEE-AE33-1C4C-816E-48B5D61F896D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC7D457-9A90-EA49-A31C-77ACF300CBDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="500" windowWidth="30060" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="800" yWindow="740" windowWidth="28000" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="131">
   <si>
     <t>Religion</t>
   </si>
@@ -417,36 +417,6 @@
     <t>Trials per block</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">lincoln.jpeg
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>[Chad, can you send me these images?]
-SOME FILES STATE USING TEXT NAMES RATHER THAN IMAGES? WAS THERE A MIX?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">hitler.jpeg
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>[Chad, can you send me these images?]
-SOME FILES STATE USING TEXT NAMES RATHER THAN IMAGES? WAS THERE A MIX?</t>
-    </r>
-  </si>
-  <si>
     <t>gentle
 sensitive
 emotional
@@ -504,23 +474,6 @@
     <t>Now please respond AS IF  living is painful and dying will be pleasant</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">TRUE
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>Chad, could you confirm that you used TRUE and FALSE as response options in all your studies?</t>
-    </r>
-  </si>
-  <si>
-    <t>Chad, could you enter the year of data collection for each study?</t>
-  </si>
-  <si>
     <t>Data published</t>
   </si>
   <si>
@@ -533,27 +486,6 @@
     <t>Hussey, Barnes-Holmes, &amp; Booth (2016) Individuals with current suicidal ideation demonstrate implicit 'fearlessness of death'</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>Convenience sample of undergraduate students at an midwestern university in the United States. Course credit was offered for participation.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve">
-Chad, could you correct his description if necessary? </t>
-    </r>
-  </si>
-  <si>
-    <t>Convenience sample of undergraduate students at an midwestern university in the United States. Course credit was offered for participation.</t>
-  </si>
-  <si>
     <t>Sample 1</t>
   </si>
   <si>
@@ -570,47 +502,6 @@
   </si>
   <si>
     <t>NA</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve">NA
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Chad, could you list the reference for any publications that use this actual data?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>NA</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Chad, could you list any publications of yours that employ this IRAP? E.g., I have published studies using a death IRAP that I also have additional unpublished data for, so the measure has been published even though that data hasn't.</t>
-    </r>
   </si>
   <si>
     <t>IRAP was also used in O'Shea et al. (2016) Measuring implicit attitudes: A positive framing bias flaw in the Implicit Relational Assessment Procedure (IRAP)</t>
@@ -632,26 +523,88 @@
     <t>Similar IRAPs were employed in Barnes-Holmes et al. (2010) The Implicit Relational Assessment Procedure: Exploring the impact of private versus public contexts and the response latency criterion on pro-white and anti-black stereotyping among white Irish individuals; Power et al. (2017) Exploring Racial Bias in a European Country with a Recent History of Immigration of Black Africans; Power et al. (2017) Combining the implicit Relational Assessment Procedure and the recording of event related potentials in the analysis of racial bias: A preliminary study; and Dunne et al. (2018) Faking a race IRAP effect in the context of single versus multiple label stimuli</t>
   </si>
   <si>
-    <t>Drake et al. (2015) Exploring the reliability and convergent validity of implicit racial evaluations</t>
-  </si>
-  <si>
-    <t>The same IRAP was employed in Drake et al. (2016) Testing the IRAP: Exploring the reliability and fakability of an idiographic approach to interpersonal attitudes</t>
-  </si>
-  <si>
-    <t>Drake et al. (2022) Comparing a Nomothetic and Idiographic Approach to Implicit Social Cognition [preprint, not peer reviewed]</t>
-  </si>
-  <si>
     <t>Drake et al. (2018) Comparing Implicit Gender Stereotypes Between Women and Men with the Implicit Relational Assessment Procedure</t>
   </si>
   <si>
     <t>A similar IRAP was employed in Cartwright et al. (2016) An investigation into the relationship between the gender binary and occupational discrimination using the Implicit Relational Assessment Procedure</t>
+  </si>
+  <si>
+    <t>2012-2013</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drake, C. E., Seymour, K., &amp; Habib, R. (2016). Testing the IRAP: Exploring the reliability and fakability of an idiographic approach to interpersonal attitudes. The Psychological Record, 66, 153-163. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Drake, C. E., Sain, T., &amp; Thompson, I. (2022). Comparing a nomothetic and idiographic approach to implicit social cognition. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Preprints.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> https://psyarxiv.com/wn9b3/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Drake, C. E., Kramer, S., Sain, T., Swiatek, R., Kohn, K., &amp; Murphy, M. (2015). Exploring the reliability and convergent validity of implicit racial evaluations. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Behavior and Social Issues, 24, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>68-87.</t>
+    </r>
+  </si>
+  <si>
+    <t>Convenience sample of undergraduate psychology students at an midwestern university in the United States. Course credit was offered for participation.</t>
+  </si>
+  <si>
+    <t>lincoln.jpeg</t>
+  </si>
+  <si>
+    <t>hitler.jpeg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -683,13 +636,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -699,26 +645,49 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri (Body)"/>
     </font>
     <font>
       <sz val="12"/>
-      <name val="Calibri (Body)"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -863,7 +832,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -871,30 +840,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -905,51 +855,57 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="131">
@@ -1424,97 +1380,97 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U3" sqref="U3"/>
+      <selection pane="topRight" activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="26"/>
+    <col min="1" max="1" width="10.83203125" style="13"/>
     <col min="2" max="3" width="24.33203125" customWidth="1"/>
-    <col min="4" max="8" width="10.83203125" style="12" customWidth="1"/>
-    <col min="9" max="11" width="14.33203125" style="13" customWidth="1"/>
+    <col min="4" max="8" width="10.83203125" style="5" customWidth="1"/>
+    <col min="9" max="11" width="14.33203125" style="6" customWidth="1"/>
     <col min="12" max="12" width="19.33203125" customWidth="1"/>
     <col min="13" max="13" width="19.83203125" customWidth="1"/>
     <col min="14" max="14" width="15.83203125" customWidth="1"/>
     <col min="15" max="15" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="16.6640625" style="13" customWidth="1"/>
-    <col min="18" max="18" width="40.1640625" style="5" customWidth="1"/>
+    <col min="16" max="17" width="16.6640625" style="17" customWidth="1"/>
+    <col min="18" max="18" width="40.1640625" style="3" customWidth="1"/>
     <col min="19" max="19" width="26.6640625" customWidth="1"/>
-    <col min="20" max="20" width="23.33203125" customWidth="1"/>
-    <col min="21" max="21" width="38.33203125" customWidth="1"/>
-    <col min="22" max="22" width="73.5" customWidth="1"/>
+    <col min="20" max="20" width="23.33203125" style="23" customWidth="1"/>
+    <col min="21" max="21" width="38.33203125" style="25" customWidth="1"/>
+    <col min="22" max="22" width="73.5" style="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="25" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:22" s="12" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="F1" s="23" t="s">
+      <c r="E1" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="L1" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="M1" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="N1" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="O1" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="P1" s="23" t="s">
+      <c r="L1" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="P1" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="Q1" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="R1" s="24" t="s">
+      <c r="R1" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="S1" s="22" t="s">
+      <c r="S1" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="U1" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="V1" s="22" t="s">
-        <v>111</v>
+      <c r="T1" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="U1" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" s="20" t="s">
+        <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="136" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+    <row r="2" spans="1:22" ht="102" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1523,28 +1479,28 @@
       <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="F2" s="16" t="s">
+      <c r="E2" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="7">
         <v>80</v>
       </c>
-      <c r="H2" s="14">
+      <c r="H2" s="7">
         <v>2000</v>
       </c>
-      <c r="I2" s="15">
-        <v>3</v>
-      </c>
-      <c r="J2" s="15">
-        <v>3</v>
-      </c>
-      <c r="K2" s="15">
+      <c r="I2" s="7">
+        <v>3</v>
+      </c>
+      <c r="J2" s="7">
+        <v>3</v>
+      </c>
+      <c r="K2" s="7">
         <v>24</v>
       </c>
       <c r="L2" s="1" t="s">
@@ -1553,136 +1509,138 @@
       <c r="M2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="P2" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q2" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="R2" s="5" t="s">
+      <c r="P2" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="R2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="S2" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="T2" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="U2" s="30" t="s">
+      <c r="S2" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="T2" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="V2" s="30" t="s">
-        <v>123</v>
+      <c r="U2" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="V2" s="22" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="104" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="F3" s="18" t="s">
+      <c r="E3" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="7">
         <v>78</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="7">
         <v>2000</v>
       </c>
-      <c r="I3" s="15">
-        <v>3</v>
-      </c>
-      <c r="J3" s="15">
-        <v>3</v>
-      </c>
-      <c r="K3" s="15">
+      <c r="I3" s="7">
+        <v>3</v>
+      </c>
+      <c r="J3" s="7">
+        <v>3</v>
+      </c>
+      <c r="K3" s="7">
         <v>24</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="P3" s="20" t="b">
+      <c r="P3" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="Q3" s="20" t="b">
+      <c r="Q3" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="R3" s="11" t="s">
+      <c r="R3" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="S3" s="8" t="s">
+      <c r="S3" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="T3" s="23">
+        <v>2016</v>
+      </c>
+      <c r="U3" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="T3" s="4"/>
-      <c r="U3" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="V3" s="8" t="s">
-        <v>121</v>
+      <c r="V3" s="18" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="114" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="11" t="s">
         <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="7">
+        <v>80</v>
+      </c>
+      <c r="H4" s="7">
+        <v>2000</v>
+      </c>
+      <c r="I4" s="7">
+        <v>3</v>
+      </c>
+      <c r="J4" s="7">
+        <v>3</v>
+      </c>
+      <c r="K4" s="7">
+        <v>24</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="14">
-        <v>80</v>
-      </c>
-      <c r="H4" s="14">
-        <v>2000</v>
-      </c>
-      <c r="I4" s="15">
-        <v>3</v>
-      </c>
-      <c r="J4" s="15">
-        <v>3</v>
-      </c>
-      <c r="K4" s="15">
-        <v>24</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>36</v>
@@ -1693,30 +1651,30 @@
       <c r="O4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="P4" s="18" t="b">
+      <c r="P4" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="Q4" s="18" t="b">
+      <c r="Q4" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="R4" s="11" t="s">
+      <c r="R4" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="S4" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="T4" s="11">
+      <c r="S4" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="T4" s="23">
         <v>2013</v>
       </c>
-      <c r="U4" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="V4" s="10" t="s">
-        <v>120</v>
+      <c r="U4" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="V4" s="18" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="104" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="11" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1725,28 +1683,28 @@
       <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="F5" s="16" t="s">
+      <c r="E5" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="7">
         <v>80</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="7">
         <v>2000</v>
       </c>
-      <c r="I5" s="15">
-        <v>3</v>
-      </c>
-      <c r="J5" s="15">
-        <v>3</v>
-      </c>
-      <c r="K5" s="15">
+      <c r="I5" s="7">
+        <v>3</v>
+      </c>
+      <c r="J5" s="7">
+        <v>3</v>
+      </c>
+      <c r="K5" s="7">
         <v>24</v>
       </c>
       <c r="L5" s="1" t="s">
@@ -1761,60 +1719,60 @@
       <c r="O5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="P5" s="18" t="b">
+      <c r="P5" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="Q5" s="18" t="b">
+      <c r="Q5" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="R5" s="11" t="s">
+      <c r="R5" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="S5" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="T5" s="11">
+      <c r="S5" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="T5" s="23">
         <v>2013</v>
       </c>
-      <c r="U5" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="V5" s="10" t="s">
-        <v>121</v>
+      <c r="U5" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="V5" s="18" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="104" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D6" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="F6" s="16" t="s">
+      <c r="E6" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="7">
         <v>80</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="7">
         <v>2000</v>
       </c>
-      <c r="I6" s="15">
-        <v>3</v>
-      </c>
-      <c r="J6" s="15">
-        <v>3</v>
-      </c>
-      <c r="K6" s="15">
+      <c r="I6" s="7">
+        <v>3</v>
+      </c>
+      <c r="J6" s="7">
+        <v>3</v>
+      </c>
+      <c r="K6" s="7">
         <v>24</v>
       </c>
       <c r="L6" s="1" t="s">
@@ -1829,30 +1787,30 @@
       <c r="O6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="P6" s="18" t="b">
+      <c r="P6" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="Q6" s="18" t="b">
+      <c r="Q6" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="R6" s="11" t="s">
+      <c r="R6" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="S6" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="T6" s="11">
+      <c r="S6" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="T6" s="23">
         <v>2013</v>
       </c>
-      <c r="U6" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="V6" s="10" t="s">
-        <v>121</v>
+      <c r="U6" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="V6" s="18" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="104" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="11" t="s">
         <v>43</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1861,35 +1819,35 @@
       <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="7">
+        <v>78</v>
+      </c>
+      <c r="H7" s="7">
+        <v>2000</v>
+      </c>
+      <c r="I7" s="7">
+        <v>3</v>
+      </c>
+      <c r="J7" s="7">
+        <v>3</v>
+      </c>
+      <c r="K7" s="7">
+        <v>24</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="14">
-        <v>78</v>
-      </c>
-      <c r="H7" s="14">
-        <v>2000</v>
-      </c>
-      <c r="I7" s="15">
-        <v>3</v>
-      </c>
-      <c r="J7" s="15">
-        <v>3</v>
-      </c>
-      <c r="K7" s="15">
-        <v>24</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>50</v>
@@ -1897,94 +1855,98 @@
       <c r="O7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="P7" s="20" t="b">
+      <c r="P7" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="Q7" s="20" t="b">
+      <c r="Q7" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="R7" s="6" t="s">
+      <c r="R7" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="S7" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="T7" s="4"/>
-      <c r="U7" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="V7" s="8" t="s">
-        <v>129</v>
+      <c r="S7" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="T7" s="23">
+        <v>2013</v>
+      </c>
+      <c r="U7" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="V7" s="24" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="104" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="F8" s="18" t="s">
+      <c r="E8" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="7">
         <v>78</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="7">
         <v>2000</v>
       </c>
-      <c r="I8" s="15">
-        <v>3</v>
-      </c>
-      <c r="J8" s="15">
-        <v>3</v>
-      </c>
-      <c r="K8" s="15">
+      <c r="I8" s="7">
+        <v>3</v>
+      </c>
+      <c r="J8" s="7">
+        <v>3</v>
+      </c>
+      <c r="K8" s="7">
         <v>24</v>
       </c>
-      <c r="L8" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="N8" s="6" t="s">
+      <c r="L8" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="O8" s="6" t="s">
+      <c r="M8" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="P8" s="20" t="b">
+      <c r="N8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="P8" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="Q8" s="20" t="b">
+      <c r="Q8" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="R8" s="5" t="s">
+      <c r="R8" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="S8" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="T8" s="4"/>
-      <c r="U8" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="V8" s="8" t="s">
-        <v>132</v>
+      <c r="S8" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="T8" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="U8" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="V8" s="18" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="155" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="11" t="s">
         <v>45</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1993,35 +1955,35 @@
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="F9" s="16" t="s">
+      <c r="E9" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="8">
         <v>78</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="8">
         <v>2000</v>
       </c>
-      <c r="I9" s="18">
-        <v>3</v>
-      </c>
-      <c r="J9" s="18">
-        <v>3</v>
-      </c>
-      <c r="K9" s="18">
+      <c r="I9" s="8">
+        <v>3</v>
+      </c>
+      <c r="J9" s="8">
+        <v>3</v>
+      </c>
+      <c r="K9" s="8">
         <v>24</v>
       </c>
-      <c r="L9" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>92</v>
+      <c r="L9" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="M9" s="18" t="s">
+        <v>130</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>50</v>
@@ -2029,28 +1991,30 @@
       <c r="O9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="P9" s="18" t="b">
+      <c r="P9" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="Q9" s="18" t="b">
+      <c r="Q9" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="R9" s="6" t="s">
+      <c r="R9" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="S9" s="8" t="s">
+      <c r="S9" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="T9" s="23">
+        <v>2013</v>
+      </c>
+      <c r="U9" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="V9" s="18" t="s">
         <v>115</v>
-      </c>
-      <c r="T9" s="4"/>
-      <c r="U9" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="V9" s="8" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="104" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="11" t="s">
         <v>46</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -2059,28 +2023,28 @@
       <c r="C10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="F10" s="18" t="s">
+      <c r="E10" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="6">
         <v>80</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="6">
         <v>2000</v>
       </c>
-      <c r="I10" s="21">
-        <v>3</v>
-      </c>
-      <c r="J10" s="21">
-        <v>3</v>
-      </c>
-      <c r="K10" s="21">
+      <c r="I10" s="6">
+        <v>3</v>
+      </c>
+      <c r="J10" s="6">
+        <v>3</v>
+      </c>
+      <c r="K10" s="6">
         <v>24</v>
       </c>
       <c r="L10" s="1" t="s">
@@ -2095,30 +2059,30 @@
       <c r="O10" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="P10" s="18" t="b">
+      <c r="P10" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="Q10" s="18" t="b">
+      <c r="Q10" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="R10" s="5" t="s">
+      <c r="R10" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="S10" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="T10" s="11">
+      <c r="S10" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="T10" s="23">
         <v>2014</v>
       </c>
-      <c r="U10" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="V10" s="10" t="s">
-        <v>124</v>
+      <c r="U10" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="V10" s="18" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="104" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -2127,28 +2091,28 @@
       <c r="C11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="F11" s="16" t="s">
+      <c r="E11" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="8">
         <v>80</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="8">
         <v>2000</v>
       </c>
-      <c r="I11" s="18">
-        <v>3</v>
-      </c>
-      <c r="J11" s="18">
-        <v>3</v>
-      </c>
-      <c r="K11" s="18">
+      <c r="I11" s="8">
+        <v>3</v>
+      </c>
+      <c r="J11" s="8">
+        <v>3</v>
+      </c>
+      <c r="K11" s="8">
         <v>24</v>
       </c>
       <c r="L11" s="2" t="s">
@@ -2163,28 +2127,30 @@
       <c r="O11" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="P11" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="R11" s="5" t="s">
+      <c r="P11" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q11" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="R11" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="S11" s="8" t="s">
+      <c r="S11" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="T11" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="U11" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="V11" s="18" t="s">
         <v>115</v>
-      </c>
-      <c r="T11" s="4"/>
-      <c r="U11" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="V11" s="8" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="153" x14ac:dyDescent="0.2">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="11" t="s">
         <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2193,28 +2159,28 @@
       <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="F12" s="16" t="s">
+      <c r="E12" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="7">
         <v>80</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="7">
         <v>2000</v>
       </c>
-      <c r="I12" s="15">
-        <v>3</v>
-      </c>
-      <c r="J12" s="15">
-        <v>3</v>
-      </c>
-      <c r="K12" s="15">
+      <c r="I12" s="7">
+        <v>3</v>
+      </c>
+      <c r="J12" s="7">
+        <v>3</v>
+      </c>
+      <c r="K12" s="7">
         <v>32</v>
       </c>
       <c r="L12" s="1" t="s">
@@ -2227,32 +2193,32 @@
         <v>62</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="P12" s="18" t="b">
+        <v>117</v>
+      </c>
+      <c r="P12" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="Q12" s="18" t="b">
+      <c r="Q12" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="R12" s="5" t="s">
+      <c r="R12" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="S12" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="T12" s="29">
+      <c r="S12" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="T12" s="23">
         <v>2013</v>
       </c>
-      <c r="U12" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="V12" s="10" t="s">
-        <v>127</v>
+      <c r="U12" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="V12" s="18" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="104" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -2261,28 +2227,28 @@
       <c r="C13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="F13" s="16" t="s">
+      <c r="E13" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="16">
+      <c r="G13" s="8">
         <v>80</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="8">
         <v>2000</v>
       </c>
-      <c r="I13" s="18">
-        <v>3</v>
-      </c>
-      <c r="J13" s="18">
-        <v>3</v>
-      </c>
-      <c r="K13" s="18">
+      <c r="I13" s="8">
+        <v>3</v>
+      </c>
+      <c r="J13" s="8">
+        <v>3</v>
+      </c>
+      <c r="K13" s="8">
         <v>24</v>
       </c>
       <c r="L13" s="1" t="s">
@@ -2303,64 +2269,66 @@
       <c r="Q13" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="R13" s="5" t="s">
+      <c r="R13" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="S13" s="8" t="s">
+      <c r="S13" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="T13" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="U13" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="T13" s="4"/>
-      <c r="U13" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="V13" s="8" t="s">
-        <v>121</v>
+      <c r="V13" s="18" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:22" s="2" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="F14" s="18" t="s">
+      <c r="E14" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="8">
         <v>78</v>
       </c>
-      <c r="H14" s="18">
+      <c r="H14" s="8">
         <v>2000</v>
       </c>
-      <c r="I14" s="18">
-        <v>3</v>
-      </c>
-      <c r="J14" s="18">
-        <v>3</v>
-      </c>
-      <c r="K14" s="18">
+      <c r="I14" s="8">
+        <v>3</v>
+      </c>
+      <c r="J14" s="8">
+        <v>3</v>
+      </c>
+      <c r="K14" s="8">
         <v>24</v>
       </c>
-      <c r="L14" s="9" t="s">
+      <c r="L14" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="M14" s="9" t="s">
+      <c r="M14" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="N14" s="10" t="s">
+      <c r="N14" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="O14" s="10" t="s">
+      <c r="O14" s="4" t="s">
         <v>85</v>
       </c>
       <c r="P14" s="17" t="b">
@@ -2369,18 +2337,20 @@
       <c r="Q14" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="R14" s="5" t="s">
+      <c r="R14" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="S14" s="8" t="s">
+      <c r="S14" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="T14" s="23">
+        <v>2016</v>
+      </c>
+      <c r="U14" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="T14" s="7"/>
-      <c r="U14" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="V14" s="8" t="s">
-        <v>121</v>
+      <c r="V14" s="18" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>